<commit_message>
Updated light engine support file
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE34D5FC-D8C3-4FB1-BD02-648956B73C71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7968EC-210C-4088-B352-9626AF6FAB7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="3615" windowWidth="23040" windowHeight="8910" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="9885" yWindow="1590" windowWidth="18585" windowHeight="7770" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -255,6 +255,72 @@
   </si>
   <si>
     <t>LED-326-H00-35</t>
+  </si>
+  <si>
+    <t>LEM-198-32-3022KS</t>
+  </si>
+  <si>
+    <t>LED-198-S70-3022</t>
+  </si>
+  <si>
+    <t>LEM-219-00-6022KS</t>
+  </si>
+  <si>
+    <t>LED-219-S00-6022</t>
+  </si>
+  <si>
+    <t>LEM-236-00-35KS</t>
+  </si>
+  <si>
+    <t>LED-236-S00-35</t>
+  </si>
+  <si>
+    <t>LEM-239-00-35KS</t>
+  </si>
+  <si>
+    <t>LED-239-S00-35</t>
+  </si>
+  <si>
+    <t>LEM-240-01-35KH</t>
+  </si>
+  <si>
+    <t>LED-240-H01-35</t>
+  </si>
+  <si>
+    <t>LEM-274-00-27KH</t>
+  </si>
+  <si>
+    <t>LED-274-H00-27</t>
+  </si>
+  <si>
+    <t>LEM-274-00-30KH</t>
+  </si>
+  <si>
+    <t>LED-274-H00-30</t>
+  </si>
+  <si>
+    <t>LEM-275-32-2722KS</t>
+  </si>
+  <si>
+    <t>LED-275-S00-2722</t>
+  </si>
+  <si>
+    <t>LEM-275-32-3522KS</t>
+  </si>
+  <si>
+    <t>LED-275-S00-3522</t>
+  </si>
+  <si>
+    <t>LEM-293-00-30KH</t>
+  </si>
+  <si>
+    <t>LED-293-H00-30</t>
+  </si>
+  <si>
+    <t>LEM-313-00-3022KH</t>
+  </si>
+  <si>
+    <t>LED-313-H00-3022</t>
   </si>
 </sst>
 </file>
@@ -606,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,279 +710,367 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>24</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B48" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B37">
-    <sortCondition ref="A2:A37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B48">
+    <sortCondition ref="A1:A48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated LEM to LED file
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7968EC-210C-4088-B352-9626AF6FAB7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7202B7-B009-4FC6-AE4C-96426F9D17A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9885" yWindow="1590" windowWidth="18585" windowHeight="7770" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="13320" windowHeight="15345" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>LED-313-H00-3022</t>
+  </si>
+  <si>
+    <t>LEM-198-16-3022KH</t>
+  </si>
+  <si>
+    <t>LED-198-H35-3022</t>
   </si>
 </sst>
 </file>
@@ -672,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,383 +700,391 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>24</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B48">
-    <sortCondition ref="A1:A48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B49">
+    <sortCondition ref="A1:A49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new light engines
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7202B7-B009-4FC6-AE4C-96426F9D17A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3D37D9-6A58-475F-84D5-54B9DA826A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="13320" windowHeight="15345" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="12390" yWindow="8115" windowWidth="13320" windowHeight="7515" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -327,6 +327,204 @@
   </si>
   <si>
     <t>LED-198-H35-3022</t>
+  </si>
+  <si>
+    <t>LEM-204-00-2722KH</t>
+  </si>
+  <si>
+    <t>LEM-204-00-2722KS</t>
+  </si>
+  <si>
+    <t>LEM-204-00-3022KS</t>
+  </si>
+  <si>
+    <t>LEM-213-00-27KS</t>
+  </si>
+  <si>
+    <t>LEM-213-00-40KS</t>
+  </si>
+  <si>
+    <t>LEM-218-00-30KS</t>
+  </si>
+  <si>
+    <t>LEM-218-00-35KS</t>
+  </si>
+  <si>
+    <t>LEM-230-16-30KS</t>
+  </si>
+  <si>
+    <t>LEM-230-33-27KS</t>
+  </si>
+  <si>
+    <t>LEM-230-33-30KS</t>
+  </si>
+  <si>
+    <t>LEM-236-00-30KS</t>
+  </si>
+  <si>
+    <t>LEM-239-00-27KH</t>
+  </si>
+  <si>
+    <t>LEM-239-00-27KS</t>
+  </si>
+  <si>
+    <t>LEM-239-00-40KS</t>
+  </si>
+  <si>
+    <t>LEM-240-01-40KH</t>
+  </si>
+  <si>
+    <t>LEM-274-00-35KH</t>
+  </si>
+  <si>
+    <t>LEM-274-00-35KS</t>
+  </si>
+  <si>
+    <t>LEM-274-00-40KS</t>
+  </si>
+  <si>
+    <t>LEM-275-16-3022KH</t>
+  </si>
+  <si>
+    <t>LEM-275-32-2722KH</t>
+  </si>
+  <si>
+    <t>LEM-275-32-3022KH</t>
+  </si>
+  <si>
+    <t>LEM-281-00-2722KH</t>
+  </si>
+  <si>
+    <t>LEM-281-00-2722KS</t>
+  </si>
+  <si>
+    <t>LEM-281-00-3022KH</t>
+  </si>
+  <si>
+    <t>LEM-293-00-27KS</t>
+  </si>
+  <si>
+    <t>LEM-293-00-35KH</t>
+  </si>
+  <si>
+    <t>LEM-293-00-40KS</t>
+  </si>
+  <si>
+    <t>LEM-307-00-27KH</t>
+  </si>
+  <si>
+    <t>LEM-313-00-2722KS</t>
+  </si>
+  <si>
+    <t>LEM-313-00-3522KS</t>
+  </si>
+  <si>
+    <t>LEM-319-00-27KH</t>
+  </si>
+  <si>
+    <t>LEM-319-00-30KU</t>
+  </si>
+  <si>
+    <t>LEM-326-00-35KS</t>
+  </si>
+  <si>
+    <t>LED-204-H00-2722</t>
+  </si>
+  <si>
+    <t>LED-204-S00-2722</t>
+  </si>
+  <si>
+    <t>LED-204-S00-3022</t>
+  </si>
+  <si>
+    <t>LED-213-S00-27</t>
+  </si>
+  <si>
+    <t>LED-213-S00-40</t>
+  </si>
+  <si>
+    <t>LED-218-S00-30</t>
+  </si>
+  <si>
+    <t>LED-218-S00-35</t>
+  </si>
+  <si>
+    <t>LED-230-S01-30</t>
+  </si>
+  <si>
+    <t>LED-230-S02-27</t>
+  </si>
+  <si>
+    <t>LED-230-S02-30</t>
+  </si>
+  <si>
+    <t>LED-236-S00-30</t>
+  </si>
+  <si>
+    <t>LED-239-H00-27</t>
+  </si>
+  <si>
+    <t>LED-239-S00-27</t>
+  </si>
+  <si>
+    <t>LED-239-S00-40</t>
+  </si>
+  <si>
+    <t>LED-240-H01-40</t>
+  </si>
+  <si>
+    <t>LED-274-H00-35</t>
+  </si>
+  <si>
+    <t>LED-274-S00-35</t>
+  </si>
+  <si>
+    <t>LED-274-S00-40</t>
+  </si>
+  <si>
+    <t>LED-275-H35-3022</t>
+  </si>
+  <si>
+    <t>LED-275-H70-2722</t>
+  </si>
+  <si>
+    <t>LED-275-H00-2722</t>
+  </si>
+  <si>
+    <t>LED-281-H00-2722</t>
+  </si>
+  <si>
+    <t>LED-281-S00-2722</t>
+  </si>
+  <si>
+    <t>LED-281-H00-3022</t>
+  </si>
+  <si>
+    <t>LED-293-S00-27</t>
+  </si>
+  <si>
+    <t>LED-293-H00-35</t>
+  </si>
+  <si>
+    <t>LED-293-S00-40</t>
+  </si>
+  <si>
+    <t>LED-307-H00-27</t>
+  </si>
+  <si>
+    <t>LED-313-S00-2722</t>
+  </si>
+  <si>
+    <t>LED-313-S00-3522</t>
+  </si>
+  <si>
+    <t>LED-319-H00-27</t>
+  </si>
+  <si>
+    <t>LED-319-U00-30</t>
+  </si>
+  <si>
+    <t>LED-326-S00-35</t>
   </si>
 </sst>
 </file>
@@ -362,8 +560,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,19 +879,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -698,393 +900,749 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B24" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B30" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B33" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B35" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B37" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B38" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B40" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B41" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B43" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B44" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B45" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B46" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B47" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B48" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B54" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B56" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B57" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B62" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B64" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B67" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B68" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B69" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B71" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B72" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B75" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B76" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B78" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B79" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B80" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B82" s="1" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B49">
-    <sortCondition ref="A1:A49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B82">
+    <sortCondition ref="A2:A82"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the LEM to LED file
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9919C4-F1B6-4B22-B7BF-3A52ED81D871}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346B2F12-D89C-4E0D-9C0D-9CF62302C336}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="3915" windowWidth="18270" windowHeight="12345" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="1065" yWindow="2385" windowWidth="18270" windowHeight="12345" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -549,6 +549,9 @@
   </si>
   <si>
     <t>LED-319-U00-27</t>
+  </si>
+  <si>
+    <t>LEM-240-00-35KH</t>
   </si>
 </sst>
 </file>
@@ -903,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,6 +1699,14 @@
         <v>171</v>
       </c>
     </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B82">
     <sortCondition ref="A2:A82"/>

</xml_diff>

<commit_message>
Updated pricing on the light engines and drivers
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6E6259-8636-427D-B8A7-E218203D4D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC81102-2A5D-4F0F-AF1A-EB74CB330882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="1410" yWindow="8820" windowWidth="25815" windowHeight="7860" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="184">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -302,15 +302,9 @@
     <t>LEM-275-32-2722KS</t>
   </si>
   <si>
-    <t>LED-275-S00-2722</t>
-  </si>
-  <si>
     <t>LEM-275-32-3522KS</t>
   </si>
   <si>
-    <t>LED-275-S00-3522</t>
-  </si>
-  <si>
     <t>LEM-293-00-30KH</t>
   </si>
   <si>
@@ -488,9 +482,6 @@
     <t>LED-275-H70-2722</t>
   </si>
   <si>
-    <t>LED-275-H00-2722</t>
-  </si>
-  <si>
     <t>LED-281-H00-2722</t>
   </si>
   <si>
@@ -582,16 +573,38 @@
   </si>
   <si>
     <t>LED-397-S00-6022</t>
+  </si>
+  <si>
+    <t>LEM_Kit_Price</t>
+  </si>
+  <si>
+    <t>LED_Acct_Val</t>
+  </si>
+  <si>
+    <t>LED-275-S70-2722</t>
+  </si>
+  <si>
+    <t>LED-275-S70-3522</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -605,7 +618,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -613,14 +626,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,14 +970,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71:P72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -957,13 +991,25 @@
       <c r="B1" t="s">
         <v>37</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="C2" s="3">
+        <v>75</v>
+      </c>
+      <c r="D2" s="2">
+        <v>30.98</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -975,6 +1021,12 @@
       <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C3" s="3">
+        <v>70</v>
+      </c>
+      <c r="D3" s="2">
+        <v>30.98</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -985,6 +1037,12 @@
       <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C4" s="3">
+        <v>70</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30.98</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
@@ -995,6 +1053,12 @@
       <c r="B5" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="C5" s="3">
+        <v>70</v>
+      </c>
+      <c r="D5" s="2">
+        <v>30.98</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
@@ -1005,6 +1069,12 @@
       <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C6" s="3">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
@@ -1015,6 +1085,12 @@
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="C7" s="3">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
@@ -1025,6 +1101,12 @@
       <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="C8" s="3">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
@@ -1035,6 +1117,12 @@
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="C9" s="3">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
@@ -1045,6 +1133,12 @@
       <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C10" s="3">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
@@ -1055,25 +1149,43 @@
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C11" s="3">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2">
+        <v>14.43</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="C13" s="3">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2">
+        <v>14.42</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1085,15 +1197,27 @@
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="C14" s="3">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2">
+        <v>14.43</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+      <c r="C15" s="3">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14.43</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1105,6 +1229,12 @@
       <c r="B16" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C16" s="3">
+        <v>40</v>
+      </c>
+      <c r="D16" s="2">
+        <v>17.55</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
@@ -1115,15 +1245,27 @@
       <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="C17" s="2">
+        <v>75</v>
+      </c>
+      <c r="D17" s="2">
+        <v>21.5</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+      <c r="C18" s="3">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2">
+        <v>11.7</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1135,6 +1277,12 @@
       <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C19" s="3">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
@@ -1145,35 +1293,59 @@
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="C20" s="3">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2">
+        <v>11.7</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="C21" s="3">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2">
+        <v>11.7</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
+      </c>
+      <c r="C22" s="3">
+        <v>90</v>
+      </c>
+      <c r="D22" s="2">
+        <v>39.85</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="C23" s="3">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2">
+        <v>39.85</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1185,602 +1357,1016 @@
       <c r="B24" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="C24" s="3">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2">
+        <v>20.100000000000001</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="C25" s="3">
+        <v>55</v>
+      </c>
+      <c r="D25" s="2">
+        <v>24.69</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>139</v>
+      <c r="A26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="3">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2">
+        <v>24.69</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="C27" s="3">
+        <v>55</v>
+      </c>
+      <c r="D27" s="2">
+        <v>24.69</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="3">
         <v>55</v>
+      </c>
+      <c r="D28" s="2">
+        <v>24.69</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>141</v>
+        <v>55</v>
+      </c>
+      <c r="C29" s="3">
+        <v>135</v>
+      </c>
+      <c r="D29" s="2">
+        <v>68</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>139</v>
+      </c>
+      <c r="C30" s="3">
+        <v>90</v>
+      </c>
+      <c r="D30" s="2">
+        <v>41.09</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>142</v>
+        <v>79</v>
+      </c>
+      <c r="C31" s="3">
+        <v>90</v>
+      </c>
+      <c r="D31" s="2">
+        <v>41.09</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2">
+        <v>13.8</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>141</v>
+      </c>
+      <c r="C33" s="3">
+        <v>40</v>
+      </c>
+      <c r="D33" s="2">
+        <v>13.8</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>144</v>
+      <c r="A34" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="3">
+        <v>40</v>
+      </c>
+      <c r="D34" s="2">
+        <v>13.8</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
+      </c>
+      <c r="C35" s="3">
+        <v>40</v>
+      </c>
+      <c r="D35" s="2">
+        <v>13.8</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>142</v>
+      </c>
+      <c r="C36" s="3">
+        <v>40</v>
+      </c>
+      <c r="D36" s="2">
+        <v>13.8</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45</v>
+      </c>
+      <c r="D37" s="2">
+        <v>13.8</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="C38" s="3">
+        <v>40</v>
+      </c>
+      <c r="D38" s="2">
+        <v>13.8</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="3">
         <v>45</v>
+      </c>
+      <c r="D39" s="2">
+        <v>13.8</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="C40" s="3">
+        <v>40</v>
+      </c>
+      <c r="D40" s="2">
+        <v>13.8</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>82</v>
+      <c r="A41" t="s">
+        <v>169</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="C41" s="3">
+        <v>45</v>
+      </c>
+      <c r="D41" s="2">
+        <v>13.8</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>145</v>
+        <v>45</v>
+      </c>
+      <c r="C42" s="3">
+        <v>40</v>
+      </c>
+      <c r="D42" s="2">
+        <v>13.8</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="C43" s="3">
+        <v>40</v>
+      </c>
+      <c r="D43" s="2">
+        <v>13.8</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>57</v>
+        <v>83</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45</v>
+      </c>
+      <c r="D44" s="2">
+        <v>13.8</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>85</v>
+        <v>143</v>
+      </c>
+      <c r="C45" s="3">
+        <v>45</v>
+      </c>
+      <c r="D45" s="2">
+        <v>13.8</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
+      </c>
+      <c r="C46" s="3">
+        <v>45</v>
+      </c>
+      <c r="D46" s="2">
+        <v>13.69</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>87</v>
+        <v>57</v>
+      </c>
+      <c r="C47" s="3">
+        <v>90</v>
+      </c>
+      <c r="D47" s="2">
+        <v>44</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="3">
+        <v>35</v>
+      </c>
+      <c r="D48" s="2">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="3">
+        <v>30</v>
+      </c>
+      <c r="D49" s="2">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="3">
+        <v>35</v>
+      </c>
+      <c r="D50" s="2">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="C51" s="3">
+        <v>30</v>
+      </c>
+      <c r="D51" s="2">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="3">
+        <v>35</v>
+      </c>
+      <c r="D52" s="2">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="3">
+        <v>30</v>
+      </c>
+      <c r="D53" s="2">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="C54" s="3">
+        <v>30</v>
+      </c>
+      <c r="D54" s="2">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" s="2">
+        <v>61</v>
+      </c>
+      <c r="D55" s="2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="C56" s="3">
+        <v>65</v>
+      </c>
+      <c r="D56" s="2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="C57" s="3">
+        <v>65</v>
+      </c>
+      <c r="D57" s="2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" s="3">
+        <v>60</v>
+      </c>
+      <c r="D58" s="2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="3">
+        <v>65</v>
+      </c>
+      <c r="D59" s="2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="3">
+        <v>60</v>
+      </c>
+      <c r="D60" s="2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="3">
+        <v>60</v>
+      </c>
+      <c r="D61" s="2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="C62" s="3">
+        <v>35</v>
+      </c>
+      <c r="D62" s="2">
+        <v>11.85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="C63" s="3">
+        <v>30</v>
+      </c>
+      <c r="D63" s="2">
+        <v>11.55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="C64" s="3">
+        <v>35</v>
+      </c>
+      <c r="D64" s="2">
+        <v>11.85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="3">
+        <v>65</v>
+      </c>
+      <c r="D65" s="2">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="C66" s="3">
+        <v>70</v>
+      </c>
+      <c r="D66" s="2">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>162</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="3">
+        <v>65</v>
+      </c>
+      <c r="D67" s="2">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="C68" s="3">
+        <v>70</v>
+      </c>
+      <c r="D68" s="2">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="3">
+        <v>65</v>
+      </c>
+      <c r="D69" s="2">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="C70" s="3">
+        <v>65</v>
+      </c>
+      <c r="D70" s="2">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="C71" s="3">
+        <v>25</v>
+      </c>
+      <c r="D71" s="2">
+        <v>2.8355999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" s="3">
+        <v>25</v>
+      </c>
+      <c r="D72" s="2">
+        <v>2.8355999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C73" s="3">
+        <v>20</v>
+      </c>
+      <c r="D73" s="2">
+        <v>2.8355999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>163</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="2">
+        <v>25</v>
+      </c>
+      <c r="D74" s="2">
+        <v>2.8355999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C75" s="3">
+        <v>20</v>
+      </c>
+      <c r="D75" s="2">
+        <v>2.8355999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="3">
+        <v>60</v>
+      </c>
+      <c r="D76" s="2">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="C77" s="3">
+        <v>65</v>
+      </c>
+      <c r="D77" s="2">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="D78" s="2">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="C79" s="3">
+        <v>60</v>
+      </c>
+      <c r="D79" s="2">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="C80" s="3">
+        <v>40</v>
+      </c>
+      <c r="D80" s="2">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>164</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="3">
+        <v>35</v>
+      </c>
+      <c r="D81" s="2">
+        <v>10.55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" s="3">
+        <v>40</v>
+      </c>
+      <c r="D82" s="2">
+        <v>10.55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" s="3">
+        <v>35</v>
+      </c>
+      <c r="D83" s="2">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B73" s="1" t="s">
+      <c r="C84" s="3">
+        <v>35</v>
+      </c>
+      <c r="D84" s="2">
+        <v>10.55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" s="3">
+        <v>40</v>
+      </c>
+      <c r="D85" s="2">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86" s="3">
+        <v>35</v>
+      </c>
+      <c r="D86" s="2">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" s="3">
+        <v>35</v>
+      </c>
+      <c r="D87" s="2">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C88" s="3">
+        <v>35</v>
+      </c>
+      <c r="D88" s="2">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="2">
+        <v>28</v>
+      </c>
+      <c r="D89" s="2">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="C90" s="3">
         <v>35</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="D90" s="2">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>164</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>165</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>166</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>167</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>172</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>173</v>
-      </c>
-      <c r="B88" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>175</v>
-      </c>
-      <c r="B89" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="C91" s="3">
+        <v>35</v>
+      </c>
+      <c r="D91" s="2">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>177</v>
       </c>
-      <c r="B90" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B92" t="s">
         <v>179</v>
       </c>
-      <c r="B91" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>180</v>
-      </c>
-      <c r="B92" t="s">
-        <v>182</v>
+      <c r="C92" s="2">
+        <v>43</v>
+      </c>
+      <c r="D92" s="2">
+        <v>20.100000000000001</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B82">
-    <sortCondition ref="A2:A82"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D92">
+    <sortCondition ref="A2:A92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated prices for drivers and LEDS
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC81102-2A5D-4F0F-AF1A-EB74CB330882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A051E3A-7475-4B09-85E3-8D902D201EDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="8820" windowWidth="25815" windowHeight="7860" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="18210" windowHeight="11565" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,9 +575,6 @@
     <t>LED-397-S00-6022</t>
   </si>
   <si>
-    <t>LEM_Kit_Price</t>
-  </si>
-  <si>
     <t>LED_Acct_Val</t>
   </si>
   <si>
@@ -585,6 +582,9 @@
   </si>
   <si>
     <t>LED-275-S70-3522</t>
+  </si>
+  <si>
+    <t>LEM_Acct_Val</t>
   </si>
 </sst>
 </file>
@@ -968,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,10 +981,10 @@
     <col min="3" max="3" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -992,13 +992,13 @@
         <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>94</v>
       </c>
@@ -1006,15 +1006,14 @@
         <v>95</v>
       </c>
       <c r="C2" s="3">
-        <v>75</v>
+        <v>32.889000000000003</v>
       </c>
       <c r="D2" s="2">
         <v>30.98</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1022,15 +1021,14 @@
         <v>47</v>
       </c>
       <c r="C3" s="3">
-        <v>70</v>
+        <v>32.889000000000003</v>
       </c>
       <c r="D3" s="2">
         <v>30.98</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1038,15 +1036,14 @@
         <v>48</v>
       </c>
       <c r="C4" s="3">
-        <v>70</v>
+        <v>32.889000000000003</v>
       </c>
       <c r="D4" s="2">
         <v>30.98</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -1054,15 +1051,14 @@
         <v>75</v>
       </c>
       <c r="C5" s="3">
-        <v>70</v>
+        <v>32.889000000000003</v>
       </c>
       <c r="D5" s="2">
         <v>30.98</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1070,15 +1066,14 @@
         <v>49</v>
       </c>
       <c r="C6" s="3">
-        <v>35</v>
+        <v>12.3874</v>
       </c>
       <c r="D6" s="2">
         <v>11.7</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1086,15 +1081,14 @@
         <v>41</v>
       </c>
       <c r="C7" s="3">
-        <v>30</v>
+        <v>12.561199999999999</v>
       </c>
       <c r="D7" s="2">
         <v>11.7</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1102,15 +1096,14 @@
         <v>50</v>
       </c>
       <c r="C8" s="3">
-        <v>35</v>
+        <v>12.3874</v>
       </c>
       <c r="D8" s="2">
         <v>11.7</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1118,15 +1111,14 @@
         <v>39</v>
       </c>
       <c r="C9" s="3">
-        <v>30</v>
+        <v>12.561199999999999</v>
       </c>
       <c r="D9" s="2">
         <v>11.7</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1134,15 +1126,14 @@
         <v>38</v>
       </c>
       <c r="C10" s="3">
-        <v>30</v>
+        <v>12.561199999999999</v>
       </c>
       <c r="D10" s="2">
         <v>11.7</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1150,15 +1141,14 @@
         <v>40</v>
       </c>
       <c r="C11" s="3">
-        <v>30</v>
+        <v>12.561199999999999</v>
       </c>
       <c r="D11" s="2">
         <v>11.7</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>96</v>
       </c>
@@ -1166,15 +1156,14 @@
         <v>129</v>
       </c>
       <c r="C12" s="3">
-        <v>45</v>
+        <v>15.055</v>
       </c>
       <c r="D12" s="2">
         <v>14.43</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>97</v>
       </c>
@@ -1182,15 +1171,14 @@
         <v>130</v>
       </c>
       <c r="C13" s="3">
-        <v>40</v>
+        <v>15.045</v>
       </c>
       <c r="D13" s="2">
         <v>14.42</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1198,15 +1186,14 @@
         <v>51</v>
       </c>
       <c r="C14" s="3">
-        <v>45</v>
+        <v>15.2288</v>
       </c>
       <c r="D14" s="2">
         <v>14.43</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -1214,15 +1201,14 @@
         <v>131</v>
       </c>
       <c r="C15" s="3">
-        <v>40</v>
+        <v>15.146699999999999</v>
       </c>
       <c r="D15" s="2">
         <v>14.43</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1230,15 +1216,14 @@
         <v>52</v>
       </c>
       <c r="C16" s="3">
-        <v>40</v>
+        <v>18.2667</v>
       </c>
       <c r="D16" s="2">
         <v>17.55</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1246,15 +1231,14 @@
         <v>53</v>
       </c>
       <c r="C17" s="2">
-        <v>75</v>
+        <v>23.408999999999999</v>
       </c>
       <c r="D17" s="2">
         <v>21.5</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>99</v>
       </c>
@@ -1262,15 +1246,14 @@
         <v>132</v>
       </c>
       <c r="C18" s="3">
-        <v>30</v>
+        <v>13.609</v>
       </c>
       <c r="D18" s="2">
         <v>11.7</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1278,15 +1261,14 @@
         <v>54</v>
       </c>
       <c r="C19" s="3">
-        <v>30</v>
+        <v>13.609</v>
       </c>
       <c r="D19" s="2">
         <v>11.7</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1294,15 +1276,14 @@
         <v>43</v>
       </c>
       <c r="C20" s="3">
-        <v>30</v>
+        <v>13.609</v>
       </c>
       <c r="D20" s="2">
         <v>11.7</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>100</v>
       </c>
@@ -1310,15 +1291,14 @@
         <v>133</v>
       </c>
       <c r="C21" s="3">
-        <v>30</v>
+        <v>13.609</v>
       </c>
       <c r="D21" s="2">
         <v>11.7</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>101</v>
       </c>
@@ -1326,15 +1306,14 @@
         <v>134</v>
       </c>
       <c r="C22" s="3">
-        <v>90</v>
+        <v>42.3491</v>
       </c>
       <c r="D22" s="2">
         <v>39.85</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>102</v>
       </c>
@@ -1342,15 +1321,14 @@
         <v>135</v>
       </c>
       <c r="C23" s="3">
-        <v>90</v>
+        <v>42.3491</v>
       </c>
       <c r="D23" s="2">
         <v>39.85</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -1358,15 +1336,14 @@
         <v>77</v>
       </c>
       <c r="C24" s="3">
-        <v>60</v>
+        <v>20.725000000000001</v>
       </c>
       <c r="D24" s="2">
         <v>20.100000000000001</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>103</v>
       </c>
@@ -1374,15 +1351,14 @@
         <v>136</v>
       </c>
       <c r="C25" s="3">
-        <v>55</v>
+        <v>26.599</v>
       </c>
       <c r="D25" s="2">
         <v>24.69</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -1390,15 +1366,14 @@
         <v>171</v>
       </c>
       <c r="C26" s="3">
-        <v>60</v>
+        <v>26.599</v>
       </c>
       <c r="D26" s="2">
         <v>24.69</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
@@ -1406,15 +1381,14 @@
         <v>137</v>
       </c>
       <c r="C27" s="3">
-        <v>55</v>
+        <v>26.599</v>
       </c>
       <c r="D27" s="2">
         <v>24.69</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
@@ -1422,15 +1396,14 @@
         <v>138</v>
       </c>
       <c r="C28" s="3">
-        <v>55</v>
+        <v>26.599</v>
       </c>
       <c r="D28" s="2">
         <v>24.69</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1438,15 +1411,14 @@
         <v>55</v>
       </c>
       <c r="C29" s="3">
-        <v>135</v>
+        <v>70.499099999999999</v>
       </c>
       <c r="D29" s="2">
         <v>68</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>106</v>
       </c>
@@ -1454,15 +1426,14 @@
         <v>139</v>
       </c>
       <c r="C30" s="3">
-        <v>90</v>
+        <v>41.808100000000003</v>
       </c>
       <c r="D30" s="2">
         <v>41.09</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>78</v>
       </c>
@@ -1470,15 +1441,14 @@
         <v>79</v>
       </c>
       <c r="C31" s="3">
-        <v>90</v>
+        <v>41.808100000000003</v>
       </c>
       <c r="D31" s="2">
         <v>41.09</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>107</v>
       </c>
@@ -1486,15 +1456,14 @@
         <v>140</v>
       </c>
       <c r="C32" s="3">
-        <v>45</v>
+        <v>15.6265</v>
       </c>
       <c r="D32" s="2">
         <v>13.8</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
@@ -1502,15 +1471,14 @@
         <v>141</v>
       </c>
       <c r="C33" s="3">
-        <v>40</v>
+        <v>15.6265</v>
       </c>
       <c r="D33" s="2">
         <v>13.8</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>176</v>
       </c>
@@ -1518,15 +1486,14 @@
         <v>178</v>
       </c>
       <c r="C34" s="3">
-        <v>40</v>
+        <v>15.6265</v>
       </c>
       <c r="D34" s="2">
         <v>13.8</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -1534,15 +1501,14 @@
         <v>81</v>
       </c>
       <c r="C35" s="3">
-        <v>40</v>
+        <v>15.6265</v>
       </c>
       <c r="D35" s="2">
         <v>13.8</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>109</v>
       </c>
@@ -1550,15 +1516,14 @@
         <v>142</v>
       </c>
       <c r="C36" s="3">
-        <v>40</v>
+        <v>15.6265</v>
       </c>
       <c r="D36" s="2">
         <v>13.8</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
@@ -1566,15 +1531,14 @@
         <v>61</v>
       </c>
       <c r="C37" s="3">
-        <v>45</v>
+        <v>15.709</v>
       </c>
       <c r="D37" s="2">
         <v>13.8</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -1582,15 +1546,14 @@
         <v>56</v>
       </c>
       <c r="C38" s="3">
-        <v>40</v>
+        <v>15.709</v>
       </c>
       <c r="D38" s="2">
         <v>13.8</v>
       </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1598,15 +1561,14 @@
         <v>62</v>
       </c>
       <c r="C39" s="3">
-        <v>45</v>
+        <v>15.709</v>
       </c>
       <c r="D39" s="2">
         <v>13.8</v>
       </c>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
@@ -1614,15 +1576,14 @@
         <v>46</v>
       </c>
       <c r="C40" s="3">
-        <v>40</v>
+        <v>15.709</v>
       </c>
       <c r="D40" s="2">
         <v>13.8</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>169</v>
       </c>
@@ -1630,15 +1591,14 @@
         <v>83</v>
       </c>
       <c r="C41" s="3">
-        <v>45</v>
+        <v>15.709</v>
       </c>
       <c r="D41" s="2">
         <v>13.8</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1646,15 +1606,14 @@
         <v>45</v>
       </c>
       <c r="C42" s="3">
-        <v>40</v>
+        <v>15.709</v>
       </c>
       <c r="D42" s="2">
         <v>13.8</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1662,15 +1621,14 @@
         <v>44</v>
       </c>
       <c r="C43" s="3">
-        <v>40</v>
+        <v>15.709</v>
       </c>
       <c r="D43" s="2">
         <v>13.8</v>
       </c>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
@@ -1678,15 +1636,14 @@
         <v>83</v>
       </c>
       <c r="C44" s="3">
-        <v>45</v>
+        <v>15.709</v>
       </c>
       <c r="D44" s="2">
         <v>13.8</v>
       </c>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>110</v>
       </c>
@@ -1694,15 +1651,14 @@
         <v>143</v>
       </c>
       <c r="C45" s="3">
-        <v>45</v>
+        <v>15.709</v>
       </c>
       <c r="D45" s="2">
         <v>13.8</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>31</v>
       </c>
@@ -1710,15 +1666,14 @@
         <v>63</v>
       </c>
       <c r="C46" s="3">
-        <v>45</v>
+        <v>15.1526</v>
       </c>
       <c r="D46" s="2">
         <v>13.69</v>
       </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>22</v>
       </c>
@@ -1726,15 +1681,14 @@
         <v>57</v>
       </c>
       <c r="C47" s="3">
-        <v>90</v>
+        <v>45.908999999999999</v>
       </c>
       <c r="D47" s="2">
         <v>44</v>
       </c>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>84</v>
       </c>
@@ -1742,7 +1696,7 @@
         <v>85</v>
       </c>
       <c r="C48" s="3">
-        <v>35</v>
+        <v>12.342599999999999</v>
       </c>
       <c r="D48" s="2">
         <v>10.82</v>
@@ -1756,7 +1710,7 @@
         <v>58</v>
       </c>
       <c r="C49" s="3">
-        <v>30</v>
+        <v>12.342599999999999</v>
       </c>
       <c r="D49" s="2">
         <v>10.82</v>
@@ -1770,7 +1724,7 @@
         <v>87</v>
       </c>
       <c r="C50" s="3">
-        <v>35</v>
+        <v>12.342599999999999</v>
       </c>
       <c r="D50" s="2">
         <v>10.82</v>
@@ -1784,7 +1738,7 @@
         <v>59</v>
       </c>
       <c r="C51" s="3">
-        <v>30</v>
+        <v>12.342599999999999</v>
       </c>
       <c r="D51" s="2">
         <v>10.82</v>
@@ -1798,7 +1752,7 @@
         <v>144</v>
       </c>
       <c r="C52" s="3">
-        <v>35</v>
+        <v>12.342599999999999</v>
       </c>
       <c r="D52" s="2">
         <v>10.82</v>
@@ -1812,7 +1766,7 @@
         <v>145</v>
       </c>
       <c r="C53" s="3">
-        <v>30</v>
+        <v>12.342599999999999</v>
       </c>
       <c r="D53" s="2">
         <v>10.82</v>
@@ -1826,7 +1780,7 @@
         <v>146</v>
       </c>
       <c r="C54" s="3">
-        <v>30</v>
+        <v>12.342599999999999</v>
       </c>
       <c r="D54" s="2">
         <v>10.82</v>
@@ -1840,7 +1794,7 @@
         <v>165</v>
       </c>
       <c r="C55" s="2">
-        <v>61</v>
+        <v>29.109000000000002</v>
       </c>
       <c r="D55" s="2">
         <v>27.2</v>
@@ -1854,7 +1808,7 @@
         <v>147</v>
       </c>
       <c r="C56" s="3">
-        <v>65</v>
+        <v>29.109000000000002</v>
       </c>
       <c r="D56" s="2">
         <v>27.2</v>
@@ -1868,7 +1822,7 @@
         <v>148</v>
       </c>
       <c r="C57" s="3">
-        <v>65</v>
+        <v>29.109000000000002</v>
       </c>
       <c r="D57" s="2">
         <v>27.2</v>
@@ -1879,10 +1833,10 @@
         <v>88</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58" s="3">
-        <v>60</v>
+        <v>29.109000000000002</v>
       </c>
       <c r="D58" s="2">
         <v>27.2</v>
@@ -1896,7 +1850,7 @@
         <v>148</v>
       </c>
       <c r="C59" s="3">
-        <v>65</v>
+        <v>29.109000000000002</v>
       </c>
       <c r="D59" s="2">
         <v>27.2</v>
@@ -1910,7 +1864,7 @@
         <v>64</v>
       </c>
       <c r="C60" s="3">
-        <v>60</v>
+        <v>29.109000000000002</v>
       </c>
       <c r="D60" s="2">
         <v>27.2</v>
@@ -1921,10 +1875,10 @@
         <v>89</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C61" s="3">
-        <v>60</v>
+        <v>29.109000000000002</v>
       </c>
       <c r="D61" s="2">
         <v>27.2</v>
@@ -1938,7 +1892,7 @@
         <v>149</v>
       </c>
       <c r="C62" s="3">
-        <v>35</v>
+        <v>13.3726</v>
       </c>
       <c r="D62" s="2">
         <v>11.85</v>
@@ -1952,7 +1906,7 @@
         <v>150</v>
       </c>
       <c r="C63" s="3">
-        <v>30</v>
+        <v>13.0726</v>
       </c>
       <c r="D63" s="2">
         <v>11.55</v>
@@ -1966,7 +1920,7 @@
         <v>151</v>
       </c>
       <c r="C64" s="3">
-        <v>35</v>
+        <v>13.3726</v>
       </c>
       <c r="D64" s="2">
         <v>11.85</v>
@@ -1980,7 +1934,7 @@
         <v>152</v>
       </c>
       <c r="C65" s="3">
-        <v>65</v>
+        <v>25.859000000000002</v>
       </c>
       <c r="D65" s="2">
         <v>23.95</v>
@@ -1994,7 +1948,7 @@
         <v>91</v>
       </c>
       <c r="C66" s="3">
-        <v>70</v>
+        <v>25.859000000000002</v>
       </c>
       <c r="D66" s="2">
         <v>23.95</v>
@@ -2008,7 +1962,7 @@
         <v>166</v>
       </c>
       <c r="C67" s="3">
-        <v>65</v>
+        <v>25.859000000000002</v>
       </c>
       <c r="D67" s="2">
         <v>23.95</v>
@@ -2022,7 +1976,7 @@
         <v>153</v>
       </c>
       <c r="C68" s="3">
-        <v>70</v>
+        <v>25.859000000000002</v>
       </c>
       <c r="D68" s="2">
         <v>23.95</v>
@@ -2036,7 +1990,7 @@
         <v>60</v>
       </c>
       <c r="C69" s="3">
-        <v>65</v>
+        <v>25.859000000000002</v>
       </c>
       <c r="D69" s="2">
         <v>23.95</v>
@@ -2050,7 +2004,7 @@
         <v>154</v>
       </c>
       <c r="C70" s="3">
-        <v>65</v>
+        <v>25.859000000000002</v>
       </c>
       <c r="D70" s="2">
         <v>23.95</v>
@@ -2064,7 +2018,7 @@
         <v>155</v>
       </c>
       <c r="C71" s="3">
-        <v>25</v>
+        <v>4.1643999999999997</v>
       </c>
       <c r="D71" s="2">
         <v>2.8355999999999999</v>
@@ -2078,7 +2032,7 @@
         <v>42</v>
       </c>
       <c r="C72" s="3">
-        <v>25</v>
+        <v>4.1326999999999998</v>
       </c>
       <c r="D72" s="2">
         <v>2.8355999999999999</v>
@@ -2092,7 +2046,7 @@
         <v>65</v>
       </c>
       <c r="C73" s="3">
-        <v>20</v>
+        <v>4.1326999999999998</v>
       </c>
       <c r="D73" s="2">
         <v>2.8355999999999999</v>
@@ -2106,7 +2060,7 @@
         <v>167</v>
       </c>
       <c r="C74" s="2">
-        <v>25</v>
+        <v>4.1326999999999998</v>
       </c>
       <c r="D74" s="2">
         <v>2.8355999999999999</v>
@@ -2120,7 +2074,7 @@
         <v>66</v>
       </c>
       <c r="C75" s="3">
-        <v>20</v>
+        <v>4.1326999999999998</v>
       </c>
       <c r="D75" s="2">
         <v>2.8355999999999999</v>
@@ -2134,7 +2088,7 @@
         <v>156</v>
       </c>
       <c r="C76" s="3">
-        <v>60</v>
+        <v>25.925000000000001</v>
       </c>
       <c r="D76" s="2">
         <v>25.3</v>
@@ -2148,7 +2102,7 @@
         <v>93</v>
       </c>
       <c r="C77" s="3">
-        <v>65</v>
+        <v>25.925000000000001</v>
       </c>
       <c r="D77" s="2">
         <v>25.3</v>
@@ -2162,7 +2116,7 @@
         <v>67</v>
       </c>
       <c r="C78" s="3">
-        <v>60</v>
+        <v>25.925000000000001</v>
       </c>
       <c r="D78" s="2">
         <v>25.3</v>
@@ -2176,7 +2130,7 @@
         <v>157</v>
       </c>
       <c r="C79" s="3">
-        <v>60</v>
+        <v>25.925000000000001</v>
       </c>
       <c r="D79" s="2">
         <v>25.3</v>
@@ -2190,7 +2144,7 @@
         <v>158</v>
       </c>
       <c r="C80" s="3">
-        <v>40</v>
+        <v>11.613799999999999</v>
       </c>
       <c r="D80" s="2">
         <v>10.25</v>
@@ -2204,7 +2158,7 @@
         <v>168</v>
       </c>
       <c r="C81" s="3">
-        <v>35</v>
+        <v>11.9139</v>
       </c>
       <c r="D81" s="2">
         <v>10.55</v>
@@ -2218,7 +2172,7 @@
         <v>72</v>
       </c>
       <c r="C82" s="3">
-        <v>40</v>
+        <v>11.613899999999999</v>
       </c>
       <c r="D82" s="2">
         <v>10.55</v>
@@ -2232,7 +2186,7 @@
         <v>68</v>
       </c>
       <c r="C83" s="3">
-        <v>35</v>
+        <v>11.613899999999999</v>
       </c>
       <c r="D83" s="2">
         <v>10.25</v>
@@ -2246,7 +2200,7 @@
         <v>159</v>
       </c>
       <c r="C84" s="3">
-        <v>35</v>
+        <v>11.9139</v>
       </c>
       <c r="D84" s="2">
         <v>10.55</v>
@@ -2260,7 +2214,7 @@
         <v>173</v>
       </c>
       <c r="C85" s="3">
-        <v>40</v>
+        <v>11.613899999999999</v>
       </c>
       <c r="D85" s="2">
         <v>10.25</v>
@@ -2274,7 +2228,7 @@
         <v>69</v>
       </c>
       <c r="C86" s="3">
-        <v>35</v>
+        <v>11.613899999999999</v>
       </c>
       <c r="D86" s="2">
         <v>10.25</v>
@@ -2288,7 +2242,7 @@
         <v>175</v>
       </c>
       <c r="C87" s="3">
-        <v>35</v>
+        <v>11.808999999999999</v>
       </c>
       <c r="D87" s="2">
         <v>9.9</v>
@@ -2302,7 +2256,7 @@
         <v>70</v>
       </c>
       <c r="C88" s="3">
-        <v>35</v>
+        <v>11.808999999999999</v>
       </c>
       <c r="D88" s="2">
         <v>9.9</v>
@@ -2316,7 +2270,7 @@
         <v>73</v>
       </c>
       <c r="C89" s="2">
-        <v>28</v>
+        <v>11.808999999999999</v>
       </c>
       <c r="D89" s="2">
         <v>9.9</v>
@@ -2330,7 +2284,7 @@
         <v>160</v>
       </c>
       <c r="C90" s="3">
-        <v>35</v>
+        <v>11.808999999999999</v>
       </c>
       <c r="D90" s="2">
         <v>9.9</v>
@@ -2344,7 +2298,7 @@
         <v>71</v>
       </c>
       <c r="C91" s="3">
-        <v>35</v>
+        <v>30.475000000000001</v>
       </c>
       <c r="D91" s="2">
         <v>29.85</v>
@@ -2358,7 +2312,7 @@
         <v>179</v>
       </c>
       <c r="C92" s="2">
-        <v>43</v>
+        <v>21.463799999999999</v>
       </c>
       <c r="D92" s="2">
         <v>20.100000000000001</v>

</xml_diff>

<commit_message>
Added some new LEM kits
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A051E3A-7475-4B09-85E3-8D902D201EDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041C072-3BF5-4CA2-ACF4-C91DE7D9505F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="18210" windowHeight="11565" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="3900" yWindow="4770" windowWidth="18210" windowHeight="11565" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -585,13 +585,32 @@
   </si>
   <si>
     <t>LEM_Acct_Val</t>
+  </si>
+  <si>
+    <t>LEM-218-00-27KS</t>
+  </si>
+  <si>
+    <t>LEM-293-00-27KH</t>
+  </si>
+  <si>
+    <t>LEM-326-00-30KH</t>
+  </si>
+  <si>
+    <t>LED-218-S00-27</t>
+  </si>
+  <si>
+    <t>LED-293-H00-27</t>
+  </si>
+  <si>
+    <t>LED-326-H00-30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -645,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,6 +672,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,6 +2341,51 @@
         <v>20.100000000000001</v>
       </c>
     </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="2">
+        <v>42.3491</v>
+      </c>
+      <c r="D93" s="2">
+        <v>39.85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="2">
+        <v>25.859000000000002</v>
+      </c>
+      <c r="D94" s="2">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C95" s="2">
+        <v>11.808999999999999</v>
+      </c>
+      <c r="D95" s="2">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D92">
     <sortCondition ref="A2:A92"/>

</xml_diff>

<commit_message>
Updated driver and LED support files
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041C072-3BF5-4CA2-ACF4-C91DE7D9505F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D57880B-C655-43FD-A54C-613296712F0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="4770" windowWidth="18210" windowHeight="11565" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="2340" yWindow="1785" windowWidth="12990" windowHeight="14415" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="191">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -603,13 +603,17 @@
   </si>
   <si>
     <t>LED-326-H00-30</t>
+  </si>
+  <si>
+    <t>LEM_Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
@@ -664,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -676,6 +680,16 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,6 +1034,9 @@
       <c r="D1" s="2" t="s">
         <v>180</v>
       </c>
+      <c r="E1" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1034,7 +1051,9 @@
       <c r="D2" s="2">
         <v>30.98</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="6">
+        <v>75</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1049,7 +1068,9 @@
       <c r="D3" s="2">
         <v>30.98</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="6">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1064,7 +1085,9 @@
       <c r="D4" s="2">
         <v>30.98</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="6">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1079,7 +1102,9 @@
       <c r="D5" s="2">
         <v>30.98</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="6">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1094,7 +1119,9 @@
       <c r="D6" s="2">
         <v>11.7</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1109,7 +1136,9 @@
       <c r="D7" s="2">
         <v>11.7</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="7">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1124,7 +1153,9 @@
       <c r="D8" s="2">
         <v>11.7</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="6">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1139,7 +1170,9 @@
       <c r="D9" s="2">
         <v>11.7</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="7">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1154,7 +1187,9 @@
       <c r="D10" s="2">
         <v>11.7</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1169,7 +1204,9 @@
       <c r="D11" s="2">
         <v>11.7</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1184,7 +1221,9 @@
       <c r="D12" s="2">
         <v>14.43</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="7">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1199,7 +1238,9 @@
       <c r="D13" s="2">
         <v>14.42</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1214,7 +1255,9 @@
       <c r="D14" s="2">
         <v>14.43</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1229,7 +1272,9 @@
       <c r="D15" s="2">
         <v>14.43</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1244,7 +1289,9 @@
       <c r="D16" s="2">
         <v>17.55</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1259,7 +1306,9 @@
       <c r="D17" s="2">
         <v>21.5</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="7">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1274,7 +1323,9 @@
       <c r="D18" s="2">
         <v>11.7</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1289,7 +1340,9 @@
       <c r="D19" s="2">
         <v>11.7</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1304,7 +1357,9 @@
       <c r="D20" s="2">
         <v>11.7</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="7">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1319,7 +1374,9 @@
       <c r="D21" s="2">
         <v>11.7</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="7">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1334,7 +1391,9 @@
       <c r="D22" s="2">
         <v>39.85</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="6">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1349,7 +1408,9 @@
       <c r="D23" s="2">
         <v>39.85</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="6">
+        <v>90</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1364,7 +1425,9 @@
       <c r="D24" s="2">
         <v>20.100000000000001</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="6">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1379,7 +1442,9 @@
       <c r="D25" s="2">
         <v>24.69</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="7">
+        <v>55</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1394,7 +1459,9 @@
       <c r="D26" s="2">
         <v>24.69</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="7">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1409,7 +1476,9 @@
       <c r="D27" s="2">
         <v>24.69</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="7">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1424,7 +1493,9 @@
       <c r="D28" s="2">
         <v>24.69</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="6">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1439,7 +1510,9 @@
       <c r="D29" s="2">
         <v>68</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="6">
+        <v>135</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1454,7 +1527,9 @@
       <c r="D30" s="2">
         <v>41.09</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="7">
+        <v>90</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1469,7 +1544,9 @@
       <c r="D31" s="2">
         <v>41.09</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="6">
+        <v>90</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1484,7 +1561,9 @@
       <c r="D32" s="2">
         <v>13.8</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1499,7 +1578,9 @@
       <c r="D33" s="2">
         <v>13.8</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1514,7 +1595,9 @@
       <c r="D34" s="2">
         <v>13.8</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="7">
+        <v>40</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1529,7 +1612,9 @@
       <c r="D35" s="2">
         <v>13.8</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -1544,7 +1629,9 @@
       <c r="D36" s="2">
         <v>13.8</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1559,7 +1646,9 @@
       <c r="D37" s="2">
         <v>13.8</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="7">
+        <v>45</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1574,7 +1663,9 @@
       <c r="D38" s="2">
         <v>13.8</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1589,7 +1680,9 @@
       <c r="D39" s="2">
         <v>13.8</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1604,7 +1697,9 @@
       <c r="D40" s="2">
         <v>13.8</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1619,7 +1714,9 @@
       <c r="D41" s="2">
         <v>13.8</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -1634,7 +1731,9 @@
       <c r="D42" s="2">
         <v>13.8</v>
       </c>
-      <c r="E42" s="1"/>
+      <c r="E42" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1649,7 +1748,9 @@
       <c r="D43" s="2">
         <v>13.8</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -1664,7 +1765,9 @@
       <c r="D44" s="2">
         <v>13.8</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -1679,7 +1782,9 @@
       <c r="D45" s="2">
         <v>13.8</v>
       </c>
-      <c r="E45" s="1"/>
+      <c r="E45" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1694,7 +1799,9 @@
       <c r="D46" s="2">
         <v>13.69</v>
       </c>
-      <c r="E46" s="1"/>
+      <c r="E46" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -1709,7 +1816,9 @@
       <c r="D47" s="2">
         <v>44</v>
       </c>
-      <c r="E47" s="1"/>
+      <c r="E47" s="6">
+        <v>90</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -1724,8 +1833,11 @@
       <c r="D48" s="2">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
@@ -1738,8 +1850,11 @@
       <c r="D49" s="2">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>86</v>
       </c>
@@ -1752,8 +1867,11 @@
       <c r="D50" s="2">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>23</v>
       </c>
@@ -1766,8 +1884,11 @@
       <c r="D51" s="2">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>111</v>
       </c>
@@ -1780,8 +1901,11 @@
       <c r="D52" s="2">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>112</v>
       </c>
@@ -1794,8 +1918,11 @@
       <c r="D53" s="2">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
@@ -1808,8 +1935,11 @@
       <c r="D54" s="2">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>161</v>
       </c>
@@ -1822,8 +1952,11 @@
       <c r="D55" s="2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>114</v>
       </c>
@@ -1836,8 +1969,11 @@
       <c r="D56" s="2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>115</v>
       </c>
@@ -1850,8 +1986,11 @@
       <c r="D57" s="2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>88</v>
       </c>
@@ -1864,8 +2003,11 @@
       <c r="D58" s="2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
@@ -1878,8 +2020,11 @@
       <c r="D59" s="2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>16</v>
       </c>
@@ -1892,8 +2037,11 @@
       <c r="D60" s="2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>89</v>
       </c>
@@ -1906,8 +2054,11 @@
       <c r="D61" s="2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>117</v>
       </c>
@@ -1920,8 +2071,11 @@
       <c r="D62" s="2">
         <v>11.85</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>118</v>
       </c>
@@ -1934,8 +2088,11 @@
       <c r="D63" s="2">
         <v>11.55</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>119</v>
       </c>
@@ -1948,8 +2105,11 @@
       <c r="D64" s="2">
         <v>11.85</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>120</v>
       </c>
@@ -1962,8 +2122,11 @@
       <c r="D65" s="2">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>90</v>
       </c>
@@ -1976,8 +2139,11 @@
       <c r="D66" s="2">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>162</v>
       </c>
@@ -1990,8 +2156,11 @@
       <c r="D67" s="2">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>121</v>
       </c>
@@ -2004,8 +2173,11 @@
       <c r="D68" s="2">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>17</v>
       </c>
@@ -2018,8 +2190,11 @@
       <c r="D69" s="2">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>122</v>
       </c>
@@ -2032,8 +2207,11 @@
       <c r="D70" s="2">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>123</v>
       </c>
@@ -2046,8 +2224,11 @@
       <c r="D71" s="2">
         <v>2.8355999999999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>1</v>
       </c>
@@ -2060,8 +2241,11 @@
       <c r="D72" s="2">
         <v>2.8355999999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>33</v>
       </c>
@@ -2074,8 +2258,11 @@
       <c r="D73" s="2">
         <v>2.8355999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>163</v>
       </c>
@@ -2088,8 +2275,11 @@
       <c r="D74" s="2">
         <v>2.8355999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>12</v>
       </c>
@@ -2102,8 +2292,11 @@
       <c r="D75" s="2">
         <v>2.8355999999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>124</v>
       </c>
@@ -2116,8 +2309,11 @@
       <c r="D76" s="2">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>92</v>
       </c>
@@ -2130,8 +2326,11 @@
       <c r="D77" s="2">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>15</v>
       </c>
@@ -2144,8 +2343,11 @@
       <c r="D78" s="2">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>125</v>
       </c>
@@ -2158,8 +2360,11 @@
       <c r="D79" s="2">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>126</v>
       </c>
@@ -2172,8 +2377,11 @@
       <c r="D80" s="2">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>164</v>
       </c>
@@ -2186,8 +2394,11 @@
       <c r="D81" s="2">
         <v>10.55</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>34</v>
       </c>
@@ -2200,8 +2411,11 @@
       <c r="D82" s="2">
         <v>10.55</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>21</v>
       </c>
@@ -2214,8 +2428,11 @@
       <c r="D83" s="2">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>127</v>
       </c>
@@ -2228,8 +2445,11 @@
       <c r="D84" s="2">
         <v>10.55</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>172</v>
       </c>
@@ -2242,8 +2462,11 @@
       <c r="D85" s="2">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>8</v>
       </c>
@@ -2256,8 +2479,11 @@
       <c r="D86" s="2">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -2270,8 +2496,11 @@
       <c r="D87" s="2">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>19</v>
       </c>
@@ -2284,8 +2513,11 @@
       <c r="D88" s="2">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>35</v>
       </c>
@@ -2298,8 +2530,11 @@
       <c r="D89" s="2">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>128</v>
       </c>
@@ -2312,8 +2547,11 @@
       <c r="D90" s="2">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>24</v>
       </c>
@@ -2326,8 +2564,11 @@
       <c r="D91" s="2">
         <v>29.85</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -2340,8 +2581,11 @@
       <c r="D92" s="2">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -2354,8 +2598,11 @@
       <c r="D93" s="2">
         <v>39.85</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>185</v>
       </c>
@@ -2368,8 +2615,11 @@
       <c r="D94" s="2">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -2382,8 +2632,11 @@
       <c r="D95" s="2">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated driver and engine files
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC7B7E5-C3DB-4513-8998-5692BC023DBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED8686A-DE65-43E0-9F9F-3CC3492C269C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="18120" windowHeight="13125" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="3465" yWindow="4935" windowWidth="18270" windowHeight="13695" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="206">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -630,6 +630,27 @@
   </si>
   <si>
     <t>LED-401-H00-3018</t>
+  </si>
+  <si>
+    <t>LEM-240-00-22KS</t>
+  </si>
+  <si>
+    <t>LEM-250-00-A1</t>
+  </si>
+  <si>
+    <t>LEM-276-32-3022KH</t>
+  </si>
+  <si>
+    <t>LEM-307-00-27KS</t>
+  </si>
+  <si>
+    <t>LED-250-C00-A1</t>
+  </si>
+  <si>
+    <t>LED-276-H70-3022</t>
+  </si>
+  <si>
+    <t>LED-307-S00-27</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1050,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:E99"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,6 +2750,74 @@
         <v>20</v>
       </c>
     </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>199</v>
+      </c>
+      <c r="B100" t="s">
+        <v>199</v>
+      </c>
+      <c r="C100" s="2">
+        <v>15.6813</v>
+      </c>
+      <c r="D100" s="2">
+        <v>15.6813</v>
+      </c>
+      <c r="E100">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C101" s="2">
+        <v>33.480899999999998</v>
+      </c>
+      <c r="D101" s="2">
+        <v>31.599599999999999</v>
+      </c>
+      <c r="E101">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>201</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C102" s="2">
+        <v>29.135300000000001</v>
+      </c>
+      <c r="D102" s="2">
+        <v>27.2</v>
+      </c>
+      <c r="E102">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>202</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C103" s="2">
+        <v>4.1326999999999998</v>
+      </c>
+      <c r="D103" s="2">
+        <v>2.8355999999999999</v>
+      </c>
+      <c r="E103">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D92">
     <sortCondition ref="A2:A92"/>

</xml_diff>

<commit_message>
Updated driver to E2 and LEM to LED
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\supportFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\USAI\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B739AA02-86DF-4118-A061-1DB84AE0C2B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635ED9DA-4B37-4822-90AE-5A7CCF485C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="18270" windowHeight="13695" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="20550" windowHeight="11475" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="218">
   <si>
     <t>LEM-203-00-35KS</t>
   </si>
@@ -657,15 +657,43 @@
   </si>
   <si>
     <t>LED-275-H35-2722</t>
+  </si>
+  <si>
+    <t>LEM-234-00-2722KS-W1</t>
+  </si>
+  <si>
+    <t>LED-234-S00-2722</t>
+  </si>
+  <si>
+    <t>LEM-239-00-30KH</t>
+  </si>
+  <si>
+    <t>LED-239-H00-30</t>
+  </si>
+  <si>
+    <t>LEM-281-00-3022KS</t>
+  </si>
+  <si>
+    <t>LED-281-S00-3022</t>
+  </si>
+  <si>
+    <t>LEM-307-00-40KH</t>
+  </si>
+  <si>
+    <t>LED-307-H00-40</t>
+  </si>
+  <si>
+    <t>LEM-326-00-40KS</t>
+  </si>
+  <si>
+    <t>LED-326-S00-40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -719,27 +747,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1056,20 +1080,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A02595-A679-40A6-BFA3-F57629D06190}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E108" sqref="E108"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1080,13 +1104,13 @@
       <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1097,13 +1121,13 @@
       <c r="B2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>32.889000000000003</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>30.98</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>75</v>
       </c>
     </row>
@@ -1114,13 +1138,13 @@
       <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>32.889000000000003</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>30.98</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>75</v>
       </c>
     </row>
@@ -1131,13 +1155,13 @@
       <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>32.889000000000003</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>30.98</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>70</v>
       </c>
     </row>
@@ -1148,13 +1172,13 @@
       <c r="B5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>32.889000000000003</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>30.98</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>70</v>
       </c>
     </row>
@@ -1165,13 +1189,13 @@
       <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>12.3874</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>11.7</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>35</v>
       </c>
     </row>
@@ -1182,13 +1206,13 @@
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>12.561199999999999</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>11.7</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>30</v>
       </c>
     </row>
@@ -1199,13 +1223,13 @@
       <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>12.3874</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>11.7</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>35</v>
       </c>
     </row>
@@ -1216,13 +1240,13 @@
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>12.561199999999999</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>11.7</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>30</v>
       </c>
     </row>
@@ -1233,13 +1257,13 @@
       <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>12.561199999999999</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>11.7</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1250,13 +1274,13 @@
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>12.561199999999999</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>11.7</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1267,13 +1291,13 @@
       <c r="B12" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <v>15.055</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>14.43</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>45</v>
       </c>
     </row>
@@ -1284,13 +1308,13 @@
       <c r="B13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>15.045</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>14.42</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1301,13 +1325,13 @@
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>15.2288</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
         <v>14.43</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1318,13 +1342,13 @@
       <c r="B15" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>15.146699999999999</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <v>14.43</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1335,13 +1359,13 @@
       <c r="B16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="5">
         <v>18.2667</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>17.55</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1352,13 +1376,13 @@
       <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <v>23.408999999999999</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="4">
         <v>21.5</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>75</v>
       </c>
     </row>
@@ -1369,13 +1393,13 @@
       <c r="B18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <v>13.609</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
         <v>11.7</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1386,13 +1410,13 @@
       <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="5">
         <v>13.609</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>11.7</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1403,13 +1427,13 @@
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="5">
         <v>13.609</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
         <v>11.7</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>30</v>
       </c>
     </row>
@@ -1420,13 +1444,13 @@
       <c r="B21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="5">
         <v>13.609</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
         <v>11.7</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>30</v>
       </c>
     </row>
@@ -1437,13 +1461,13 @@
       <c r="B22" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="5">
         <v>42.3491</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="4">
         <v>39.85</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1454,13 +1478,13 @@
       <c r="B23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="5">
         <v>42.3491</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="4">
         <v>39.85</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1471,13 +1495,13 @@
       <c r="B24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="5">
         <v>20.725000000000001</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>60</v>
       </c>
     </row>
@@ -1488,13 +1512,13 @@
       <c r="B25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="5">
         <v>26.599</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="4">
         <v>24.69</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>55</v>
       </c>
     </row>
@@ -1505,13 +1529,13 @@
       <c r="B26" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="5">
         <v>26.599</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="4">
         <v>24.69</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>60</v>
       </c>
     </row>
@@ -1522,13 +1546,13 @@
       <c r="B27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="5">
         <v>26.599</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="4">
         <v>24.69</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>55</v>
       </c>
     </row>
@@ -1539,13 +1563,13 @@
       <c r="B28" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="5">
         <v>26.599</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="4">
         <v>24.69</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>55</v>
       </c>
     </row>
@@ -1556,13 +1580,13 @@
       <c r="B29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="5">
         <v>70.499099999999999</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="4">
         <v>68</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>135</v>
       </c>
     </row>
@@ -1573,13 +1597,13 @@
       <c r="B30" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="5">
         <v>41.808100000000003</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="4">
         <v>41.09</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>90</v>
       </c>
     </row>
@@ -1590,13 +1614,13 @@
       <c r="B31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="5">
         <v>41.808100000000003</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="4">
         <v>41.09</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1607,13 +1631,13 @@
       <c r="B32" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="5">
         <v>15.6265</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="4">
         <v>13.8</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1624,13 +1648,13 @@
       <c r="B33" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="5">
         <v>15.6265</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="4">
         <v>13.8</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1641,13 +1665,13 @@
       <c r="B34" t="s">
         <v>178</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="5">
         <v>15.6265</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="4">
         <v>13.8</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>40</v>
       </c>
     </row>
@@ -1658,13 +1682,13 @@
       <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="5">
         <v>15.6265</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="4">
         <v>13.8</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1675,13 +1699,13 @@
       <c r="B36" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="5">
         <v>15.6265</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="4">
         <v>13.8</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1692,13 +1716,13 @@
       <c r="B37" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="5">
         <v>15.709</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="4">
         <v>13.8</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>45</v>
       </c>
     </row>
@@ -1709,13 +1733,13 @@
       <c r="B38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="5">
         <v>15.709</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="4">
         <v>13.8</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1726,13 +1750,13 @@
       <c r="B39" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="5">
         <v>15.709</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="4">
         <v>13.8</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1743,13 +1767,13 @@
       <c r="B40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="5">
         <v>15.709</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="4">
         <v>13.8</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1760,13 +1784,13 @@
       <c r="B41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="5">
         <v>15.709</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="4">
         <v>13.8</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1777,13 +1801,13 @@
       <c r="B42" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="5">
         <v>15.709</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="4">
         <v>13.8</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1794,13 +1818,13 @@
       <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="5">
         <v>15.709</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="4">
         <v>13.8</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1811,13 +1835,13 @@
       <c r="B44" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="5">
         <v>15.709</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="4">
         <v>13.8</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1828,13 +1852,13 @@
       <c r="B45" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="5">
         <v>15.709</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="4">
         <v>13.8</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1845,13 +1869,13 @@
       <c r="B46" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="5">
         <v>15.1526</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="4">
         <v>13.69</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1862,13 +1886,13 @@
       <c r="B47" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="5">
         <v>45.908999999999999</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="4">
         <v>44</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1879,13 +1903,13 @@
       <c r="B48" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="5">
         <v>12.342599999999999</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="4">
         <v>10.82</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <v>35</v>
       </c>
     </row>
@@ -1896,10 +1920,10 @@
       <c r="B49" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="5">
         <v>12.342599999999999</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="4">
         <v>10.82</v>
       </c>
       <c r="E49" s="4">
@@ -1913,13 +1937,13 @@
       <c r="B50" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="5">
         <v>12.342599999999999</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="4">
         <v>10.82</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="5">
         <v>35</v>
       </c>
     </row>
@@ -1930,10 +1954,10 @@
       <c r="B51" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="5">
         <v>12.342599999999999</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="4">
         <v>10.82</v>
       </c>
       <c r="E51" s="4">
@@ -1947,13 +1971,13 @@
       <c r="B52" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="5">
         <v>12.342599999999999</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="4">
         <v>10.82</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="5">
         <v>35</v>
       </c>
     </row>
@@ -1964,13 +1988,13 @@
       <c r="B53" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="5">
         <v>12.342599999999999</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="4">
         <v>10.82</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1981,13 +2005,13 @@
       <c r="B54" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="5">
         <v>12.342599999999999</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="4">
         <v>10.82</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1998,10 +2022,10 @@
       <c r="B55" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="4">
         <v>29.109000000000002</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="4">
         <v>27.2</v>
       </c>
       <c r="E55" s="4">
@@ -2015,13 +2039,13 @@
       <c r="B56" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="5">
         <v>29.109000000000002</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="4">
         <v>27.2</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="5">
         <v>65</v>
       </c>
     </row>
@@ -2032,13 +2056,13 @@
       <c r="B57" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="5">
         <v>29.109000000000002</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="4">
         <v>27.2</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="5">
         <v>65</v>
       </c>
     </row>
@@ -2049,13 +2073,13 @@
       <c r="B58" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="5">
         <v>29.109000000000002</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="4">
         <v>27.2</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E58" s="5">
         <v>60</v>
       </c>
     </row>
@@ -2066,13 +2090,13 @@
       <c r="B59" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="5">
         <v>29.109000000000002</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="4">
         <v>27.2</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="5">
         <v>65</v>
       </c>
     </row>
@@ -2083,13 +2107,13 @@
       <c r="B60" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="5">
         <v>29.109000000000002</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="4">
         <v>27.2</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60" s="5">
         <v>60</v>
       </c>
     </row>
@@ -2100,13 +2124,13 @@
       <c r="B61" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="5">
         <v>29.109000000000002</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="4">
         <v>27.2</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="5">
         <v>60</v>
       </c>
     </row>
@@ -2117,13 +2141,13 @@
       <c r="B62" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="5">
         <v>13.3726</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="4">
         <v>11.85</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2134,13 +2158,13 @@
       <c r="B63" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="5">
         <v>13.0726</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="4">
         <v>11.55</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E63" s="5">
         <v>30</v>
       </c>
     </row>
@@ -2151,13 +2175,13 @@
       <c r="B64" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="5">
         <v>13.3726</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="4">
         <v>11.85</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E64" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2168,13 +2192,13 @@
       <c r="B65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="5">
         <v>25.859000000000002</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="4">
         <v>23.95</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E65" s="5">
         <v>65</v>
       </c>
     </row>
@@ -2185,13 +2209,13 @@
       <c r="B66" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="5">
         <v>25.859000000000002</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="4">
         <v>23.95</v>
       </c>
-      <c r="E66" s="6">
+      <c r="E66" s="5">
         <v>70</v>
       </c>
     </row>
@@ -2202,13 +2226,13 @@
       <c r="B67" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="5">
         <v>25.859000000000002</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="4">
         <v>23.95</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E67" s="5">
         <v>65</v>
       </c>
     </row>
@@ -2219,13 +2243,13 @@
       <c r="B68" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="5">
         <v>25.859000000000002</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="4">
         <v>23.95</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E68" s="5">
         <v>70</v>
       </c>
     </row>
@@ -2236,13 +2260,13 @@
       <c r="B69" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="5">
         <v>25.859000000000002</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="4">
         <v>23.95</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E69" s="5">
         <v>65</v>
       </c>
     </row>
@@ -2253,13 +2277,13 @@
       <c r="B70" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="5">
         <v>25.859000000000002</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="4">
         <v>23.95</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E70" s="5">
         <v>65</v>
       </c>
     </row>
@@ -2270,13 +2294,13 @@
       <c r="B71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="5">
         <v>4.1643999999999997</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="4">
         <v>2.8355999999999999</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E71" s="4">
         <v>25</v>
       </c>
     </row>
@@ -2287,13 +2311,13 @@
       <c r="B72" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="5">
         <v>4.1326999999999998</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="4">
         <v>2.8355999999999999</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E72" s="5">
         <v>25</v>
       </c>
     </row>
@@ -2304,13 +2328,13 @@
       <c r="B73" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="5">
         <v>4.1326999999999998</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="4">
         <v>2.8355999999999999</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E73" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2321,10 +2345,10 @@
       <c r="B74" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="4">
         <v>4.1326999999999998</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="4">
         <v>2.8355999999999999</v>
       </c>
       <c r="E74" s="4">
@@ -2338,13 +2362,13 @@
       <c r="B75" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="5">
         <v>4.1326999999999998</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="4">
         <v>2.8355999999999999</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E75" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2355,13 +2379,13 @@
       <c r="B76" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="5">
         <v>25.925000000000001</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76" s="4">
         <v>25.3</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76" s="5">
         <v>60</v>
       </c>
     </row>
@@ -2372,10 +2396,10 @@
       <c r="B77" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="5">
         <v>25.925000000000001</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77" s="4">
         <v>25.3</v>
       </c>
       <c r="E77" s="4">
@@ -2389,13 +2413,13 @@
       <c r="B78" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="5">
         <v>25.925000000000001</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78" s="4">
         <v>25.3</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78" s="5">
         <v>60</v>
       </c>
     </row>
@@ -2406,13 +2430,13 @@
       <c r="B79" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="5">
         <v>25.925000000000001</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79" s="4">
         <v>25.3</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="5">
         <v>60</v>
       </c>
     </row>
@@ -2423,13 +2447,13 @@
       <c r="B80" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="5">
         <v>11.613799999999999</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="4">
         <v>10.25</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80" s="5">
         <v>40</v>
       </c>
     </row>
@@ -2440,13 +2464,13 @@
       <c r="B81" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="5">
         <v>11.9139</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="4">
         <v>10.55</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2457,13 +2481,13 @@
       <c r="B82" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="5">
         <v>11.613899999999999</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82" s="4">
         <v>10.55</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82" s="5">
         <v>40</v>
       </c>
     </row>
@@ -2474,13 +2498,13 @@
       <c r="B83" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="5">
         <v>11.613899999999999</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83" s="4">
         <v>10.25</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2491,13 +2515,13 @@
       <c r="B84" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="5">
         <v>11.9139</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84" s="4">
         <v>10.55</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2508,13 +2532,13 @@
       <c r="B85" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="5">
         <v>11.613899999999999</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85" s="4">
         <v>10.25</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E85" s="5">
         <v>40</v>
       </c>
     </row>
@@ -2525,10 +2549,10 @@
       <c r="B86" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="5">
         <v>11.613899999999999</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="4">
         <v>10.25</v>
       </c>
       <c r="E86" s="4">
@@ -2542,13 +2566,13 @@
       <c r="B87" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="5">
         <v>11.808999999999999</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87" s="4">
         <v>9.9</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E87" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2559,13 +2583,13 @@
       <c r="B88" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="5">
         <v>11.808999999999999</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="4">
         <v>9.9</v>
       </c>
-      <c r="E88" s="6">
+      <c r="E88" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2576,10 +2600,10 @@
       <c r="B89" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="4">
         <v>11.808999999999999</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89" s="4">
         <v>9.9</v>
       </c>
       <c r="E89" s="4">
@@ -2593,13 +2617,13 @@
       <c r="B90" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="5">
         <v>11.808999999999999</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="4">
         <v>9.9</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E90" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2610,13 +2634,13 @@
       <c r="B91" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="5">
         <v>30.475000000000001</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="4">
         <v>29.85</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E91" s="5">
         <v>35</v>
       </c>
     </row>
@@ -2627,10 +2651,10 @@
       <c r="B92" t="s">
         <v>179</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92" s="4">
         <v>21.463799999999999</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="4">
         <v>20.100000000000001</v>
       </c>
       <c r="E92" s="4">
@@ -2641,16 +2665,16 @@
       <c r="A93" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93" s="4">
         <v>42.3491</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="4">
         <v>39.85</v>
       </c>
-      <c r="E93" s="6">
+      <c r="E93" s="5">
         <v>90</v>
       </c>
     </row>
@@ -2658,16 +2682,16 @@
       <c r="A94" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94" s="4">
         <v>25.859000000000002</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94" s="4">
         <v>23.95</v>
       </c>
-      <c r="E94" s="6">
+      <c r="E94" s="5">
         <v>70</v>
       </c>
     </row>
@@ -2675,16 +2699,16 @@
       <c r="A95" t="s">
         <v>186</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95" s="4">
         <v>11.808999999999999</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D95" s="4">
         <v>9.9</v>
       </c>
-      <c r="E95" s="9">
+      <c r="E95" s="7">
         <v>26</v>
       </c>
     </row>
@@ -2695,13 +2719,13 @@
       <c r="B96" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96" s="4">
         <v>32.889000000000003</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D96" s="4">
         <v>30.98</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2712,13 +2736,13 @@
       <c r="B97" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97" s="4">
         <v>4.1326999999999998</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97" s="4">
         <v>2.8355999999999999</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97" s="4">
         <v>20</v>
       </c>
     </row>
@@ -2729,13 +2753,13 @@
       <c r="B98" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98" s="4">
         <v>25.925000000000001</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D98" s="4">
         <v>25.3</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98" s="4">
         <v>65</v>
       </c>
     </row>
@@ -2746,13 +2770,13 @@
       <c r="B99" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99" s="4">
         <v>6.0400999999999998</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99" s="4">
         <v>4.7430000000000003</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99" s="4">
         <v>20</v>
       </c>
     </row>
@@ -2763,13 +2787,13 @@
       <c r="B100" t="s">
         <v>199</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100" s="4">
         <v>15.6813</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D100" s="4">
         <v>15.6813</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="4">
         <v>40</v>
       </c>
     </row>
@@ -2780,13 +2804,13 @@
       <c r="B101" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101" s="4">
         <v>33.480899999999998</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101" s="4">
         <v>31.599599999999999</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="4">
         <v>80</v>
       </c>
     </row>
@@ -2797,13 +2821,13 @@
       <c r="B102" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C102" s="2">
+      <c r="C102" s="4">
         <v>29.135300000000001</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D102" s="4">
         <v>27.2</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="4">
         <v>64</v>
       </c>
     </row>
@@ -2814,13 +2838,13 @@
       <c r="B103" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C103" s="2">
+      <c r="C103" s="4">
         <v>4.1326999999999998</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D103" s="4">
         <v>2.8355999999999999</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="4">
         <v>20</v>
       </c>
     </row>
@@ -2831,14 +2855,99 @@
       <c r="B104" t="s">
         <v>207</v>
       </c>
-      <c r="C104" s="2">
+      <c r="C104" s="4">
         <v>29.081299999999999</v>
       </c>
-      <c r="D104" s="2">
+      <c r="D104" s="4">
         <v>27.2</v>
       </c>
       <c r="E104" s="4">
         <v>65</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
+        <v>209</v>
+      </c>
+      <c r="C105" s="4">
+        <v>61.024500000000003</v>
+      </c>
+      <c r="D105" s="4">
+        <v>58.25</v>
+      </c>
+      <c r="E105" s="4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>211</v>
+      </c>
+      <c r="C106" s="4">
+        <v>15.7433</v>
+      </c>
+      <c r="D106" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="E106" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" t="s">
+        <v>213</v>
+      </c>
+      <c r="C107" s="4">
+        <v>13.1622</v>
+      </c>
+      <c r="D107" s="4">
+        <v>11.55</v>
+      </c>
+      <c r="E107" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>215</v>
+      </c>
+      <c r="C108" s="4">
+        <v>4.1516999999999999</v>
+      </c>
+      <c r="D108" s="4">
+        <v>2.8355999999999999</v>
+      </c>
+      <c r="E108" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" t="s">
+        <v>217</v>
+      </c>
+      <c r="C109" s="4">
+        <v>11.789300000000001</v>
+      </c>
+      <c r="D109" s="4">
+        <v>9.9</v>
+      </c>
+      <c r="E109" s="4">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated LEM to LED spreadsheet
</commit_message>
<xml_diff>
--- a/Code/supportFiles/LEM_to_LED.xlsx
+++ b/Code/supportFiles/LEM_to_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\USAI\Code\supportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635ED9DA-4B37-4822-90AE-5A7CCF485C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C90394-3A0B-4176-955A-44F00F1DE343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="20550" windowHeight="11475" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
+    <workbookView xWindow="825" yWindow="825" windowWidth="20550" windowHeight="13830" xr2:uid="{7AA7077D-C6EC-40E7-9300-04B9337A7343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1084,7 +1084,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>